<commit_message>
updated the project by removing unwanted and 'APIUtility'.
</commit_message>
<xml_diff>
--- a/testData/ListAllDogs_one.xlsx
+++ b/testData/ListAllDogs_one.xlsx
@@ -22,10 +22,10 @@
     <t>Request Type</t>
   </si>
   <si>
-    <t>https://dog.ceo/api/breeds/list/all</t>
+    <t>GET</t>
   </si>
   <si>
-    <t>GET</t>
+    <t>https://dog.ceo/api/breeds/list/all</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,10 +438,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="4"/>
     </row>

</xml_diff>